<commit_message>
Versão final do site
</commit_message>
<xml_diff>
--- a/documentacao/BurndownSprint3.xlsx
+++ b/documentacao/BurndownSprint3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\coral-life\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\coral-life\Entregáveis 3ª Sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -640,7 +640,6 @@
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -682,10 +681,10 @@
                   <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -756,7 +755,6 @@
                 <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -798,13 +796,13 @@
                   <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68.25</c:v>
+                  <c:v>80.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -817,9 +815,8 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -908,7 +905,9 @@
         <c:spPr>
           <a:noFill/>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -918,6 +917,11 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -954,10 +958,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2412,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="A1:F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2456,12 +2457,8 @@
       <c r="D2" s="22">
         <v>13</v>
       </c>
-      <c r="E2" s="23">
-        <v>8</v>
-      </c>
-      <c r="F2" s="23">
-        <v>0</v>
-      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -2476,12 +2473,8 @@
       <c r="D3" s="22">
         <v>8</v>
       </c>
-      <c r="E3" s="23">
-        <v>13</v>
-      </c>
-      <c r="F3" s="23">
-        <v>0</v>
-      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
@@ -2496,12 +2489,8 @@
       <c r="D4" s="22">
         <v>13</v>
       </c>
-      <c r="E4" s="23">
-        <v>8</v>
-      </c>
-      <c r="F4" s="23">
-        <v>0</v>
-      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
@@ -2514,14 +2503,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="22">
-        <v>8</v>
-      </c>
-      <c r="E5" s="22">
-        <v>13</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -2534,14 +2519,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="22">
-        <v>8</v>
-      </c>
-      <c r="E6" s="22">
-        <v>13</v>
-      </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
@@ -2556,12 +2537,8 @@
       <c r="D7" s="22">
         <v>5</v>
       </c>
-      <c r="E7" s="22">
-        <v>0</v>
-      </c>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
@@ -2576,12 +2553,8 @@
       <c r="D8" s="22">
         <v>0</v>
       </c>
-      <c r="E8" s="22">
-        <v>13</v>
-      </c>
-      <c r="F8" s="22">
-        <v>0</v>
-      </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -2596,12 +2569,8 @@
       <c r="D9" s="22">
         <v>8</v>
       </c>
-      <c r="E9" s="22">
-        <v>0</v>
-      </c>
-      <c r="F9" s="22">
-        <v>0</v>
-      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
@@ -2616,12 +2585,8 @@
       <c r="D10" s="22">
         <v>8</v>
       </c>
-      <c r="E10" s="22">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22">
-        <v>0</v>
-      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -2636,12 +2601,8 @@
       <c r="D11" s="22">
         <v>0</v>
       </c>
-      <c r="E11" s="22">
-        <v>8</v>
-      </c>
-      <c r="F11" s="22">
-        <v>5</v>
-      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -2656,12 +2617,8 @@
       <c r="D12" s="22">
         <v>0</v>
       </c>
-      <c r="E12" s="22">
-        <v>8</v>
-      </c>
-      <c r="F12" s="22">
-        <v>5</v>
-      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -2676,12 +2633,8 @@
       <c r="D13" s="22">
         <v>0</v>
       </c>
-      <c r="E13" s="22">
-        <v>3</v>
-      </c>
-      <c r="F13" s="22">
-        <v>5</v>
-      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
@@ -2696,12 +2649,8 @@
       <c r="D14" s="22">
         <v>0</v>
       </c>
-      <c r="E14" s="22">
-        <v>0</v>
-      </c>
-      <c r="F14" s="22">
-        <v>8</v>
-      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -2717,13 +2666,13 @@
       </c>
       <c r="D15" s="26">
         <f>IF(SUM(D2:D14)&gt;0,C15-(SUM(D2:D14)))</f>
-        <v>110</v>
-      </c>
-      <c r="E15" s="26">
+        <v>116</v>
+      </c>
+      <c r="E15" s="26" t="b">
         <f>IF(SUM(E2:E14)&gt;0,D15-(SUM(E2:E14)))</f>
-        <v>23</v>
-      </c>
-      <c r="F15" s="26">
+        <v>0</v>
+      </c>
+      <c r="F15" s="26" t="b">
         <f>IF(SUM(F2:F14)&gt;0,E15-(SUM(F2:F14)))</f>
         <v>0</v>
       </c>
@@ -2740,14 +2689,15 @@
         <v>170</v>
       </c>
       <c r="D16" s="28">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E16" s="28">
         <f>D16-($B$16/COUNTA($C$1:$F$1))</f>
-        <v>68.25</v>
+        <v>80.25</v>
       </c>
       <c r="F16" s="28">
-        <v>0</v>
+        <f>E16-($B$16/COUNTA($C$1:$F$1))</f>
+        <v>28.5</v>
       </c>
     </row>
   </sheetData>
@@ -2759,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>